<commit_message>
Improve dataset information display
- Fix duration calculation to handle edge cases and ensure it displays
- Sort variables alphabetically for better organization
- Simplify variable display to clean columns without button styling
- Remove scrollable container and use responsive grid layout

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/Streaming_Current_Data.xlsx
+++ b/data/Streaming_Current_Data.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Reclaim Water Flow as Percentage of Plant Influent</t>
+    <t xml:space="preserve">Reclaim Water Flow % of Plant Influent</t>
   </si>
   <si>
     <t xml:space="preserve">Reclaim Water Flow</t>
@@ -3211,7 +3211,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>